<commit_message>
ASA24 data overview & lineplot fn
</commit_message>
<xml_diff>
--- a/eg_data/VVKAJ101-105/VVKAJ_2021-11-09_7963_Tot_m_QCed_fullonly.txt.xlsx
+++ b/eg_data/VVKAJ101-105/VVKAJ_2021-11-09_7963_Tot_m_QCed_fullonly.txt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadoh\OneDrive\Documents\GitHub\dietary_patterns\eg_data\VVKAJ101-105\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AFD405D-3D06-4C81-96DA-82A358FA4713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD24C502-2FA2-486F-A8B4-7E913B71732F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30015" yWindow="-1785" windowWidth="17535" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34380" yWindow="-2250" windowWidth="13590" windowHeight="10860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>